<commit_message>
ok importar xlsx a mysql
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -20,18 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">usuario3</t>
+    <t xml:space="preserve">A</t>
   </si>
   <si>
-    <t xml:space="preserve">Nombre 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">usuario4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre 4</t>
+    <t xml:space="preserve">B</t>
   </si>
 </sst>
 </file>
@@ -139,43 +133,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>1</v>
-      </c>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>2</v>
+      <c r="B2" s="0" t="n">
+        <v>22</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>